<commit_message>
ZSS-392, ZSS-423:  * re-design and modify freeze panels control  * minor fixed  * add test cases
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue/392-freeze-render.xlsx
+++ b/zss.test/src/main/webapp/issue/392-freeze-render.xlsx
@@ -4,21 +4,42 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="120" windowWidth="19176" windowHeight="9864"/>
+    <workbookView xWindow="90" yWindow="120" windowWidth="19170" windowHeight="9870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
-    <t>aa</t>
+    <t>test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200x200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sheet4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -71,7 +92,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -79,7 +100,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -363,15 +384,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:GS200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6:L6"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:201">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="GS1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:201">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:201">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:201">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:201">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:201">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:201">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:201">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:201">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:201">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:201">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:201">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:201">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:201">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:201">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:201">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="200" spans="1:201">
+      <c r="A200">
+        <v>200</v>
+      </c>
+      <c r="GS200" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -379,17 +582,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:GS200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:201">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="GS1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:201">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:201">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:201">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:201">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:201">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:201">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:201">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:201">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:201">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:201">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:201">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:201">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:201">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:201">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:201">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="200" spans="1:201">
+      <c r="A200">
+        <v>200</v>
+      </c>
+      <c r="GS200" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -400,12 +780,391 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:GS200"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:201">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="GS1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:201">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:201">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:201">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:201">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:201">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:201">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:201">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:201">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:201">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:201">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:201">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:201">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:201">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:201">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:201">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="200" spans="1:201">
+      <c r="A200">
+        <v>200</v>
+      </c>
+      <c r="GS200" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:GS200"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:201">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="GS1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:201">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:201">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:201">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:201">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:201">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:201">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:201">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:201">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:201">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:201">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:201">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:201">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:201">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:201">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:201">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="200" spans="1:201">
+      <c r="A200">
+        <v>200</v>
+      </c>
+      <c r="GS200" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>